<commit_message>
Added a method to get active zoneset data
</commit_message>
<xml_diff>
--- a/OOP Implementation/device_password_mapping.xlsx
+++ b/OOP Implementation/device_password_mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/umagrawa/Documents/GitHub/Topology_Generator/OOP Implementation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99D6EF35-F442-6B47-8ADF-A07866BFA25E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{755CEF5C-F067-634B-AD9A-086E4F902952}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15940" xr2:uid="{FA80B913-FCBD-A442-B8A5-007A08EF9666}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
   <si>
     <t>Password</t>
   </si>
@@ -54,6 +54,21 @@
   </si>
   <si>
     <t>Management IP</t>
+  </si>
+  <si>
+    <t>10.127.125.228</t>
+  </si>
+  <si>
+    <t>10.127.125.229</t>
+  </si>
+  <si>
+    <t>10.127.125.230</t>
+  </si>
+  <si>
+    <t>10.127.125.239</t>
+  </si>
+  <si>
+    <t>nbv_12345</t>
   </si>
 </sst>
 </file>
@@ -428,10 +443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EC23E06-AECA-3A40-8DDB-F4495432B0C4}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -480,6 +495,38 @@
         <v>1</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added mongoDB support to reduce latency
</commit_message>
<xml_diff>
--- a/OOP Implementation/device_password_mapping.xlsx
+++ b/OOP Implementation/device_password_mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/umagrawa/Documents/GitHub/Topology_Generator/OOP Implementation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE5A4C0A-FF33-D145-BCF2-505404B98756}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BC26358-5B14-564C-A6E5-99528D9C2B52}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15940" xr2:uid="{FA80B913-FCBD-A442-B8A5-007A08EF9666}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="32">
   <si>
     <t>Password</t>
   </si>
@@ -117,6 +117,18 @@
   </si>
   <si>
     <t>10.127.125.237</t>
+  </si>
+  <si>
+    <t>10.127.125.221</t>
+  </si>
+  <si>
+    <t>10.127.125.220</t>
+  </si>
+  <si>
+    <t>10.127.125.238</t>
+  </si>
+  <si>
+    <t>10.127.125.222</t>
   </si>
 </sst>
 </file>
@@ -491,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EC23E06-AECA-3A40-8DDB-F4495432B0C4}">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -695,6 +707,46 @@
         <v>11</v>
       </c>
     </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>